<commit_message>
MAGMA + SLICE MASTER DOWNLOAD LINK
</commit_message>
<xml_diff>
--- a/media/SLICE/Billing/FEB 22/SLICE BILLING.xlsx
+++ b/media/SLICE/Billing/FEB 22/SLICE BILLING.xlsx
@@ -532,7 +532,7 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
@@ -586,7 +586,7 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
@@ -646,7 +646,7 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>PRAMOD-JAIPUR</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
@@ -700,7 +700,7 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
@@ -754,7 +754,7 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
@@ -808,7 +808,7 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>ANIL KUMAR PANDIT</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
@@ -862,7 +862,7 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
@@ -916,7 +916,7 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
@@ -970,7 +970,7 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>PRAMOD-JAIPUR</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
@@ -1024,7 +1024,7 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>BEENESH</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
@@ -1078,7 +1078,7 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
@@ -1132,7 +1132,7 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
@@ -1186,7 +1186,7 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
@@ -1240,7 +1240,7 @@
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MANOJ TOMAR</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
@@ -1294,7 +1294,7 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>PRAMOD-JAIPUR</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
@@ -1348,7 +1348,7 @@
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MANOJ TOMAR</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
@@ -1402,7 +1402,7 @@
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
@@ -1456,7 +1456,7 @@
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
@@ -1510,7 +1510,7 @@
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>SHAKEEL</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
@@ -1570,7 +1570,7 @@
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
@@ -1624,7 +1624,7 @@
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MANOJ TOMAR</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
@@ -1678,7 +1678,7 @@
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>PRAMOD-JAIPUR</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
@@ -1732,7 +1732,7 @@
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
@@ -1786,7 +1786,7 @@
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>PRAMOD-JAIPUR</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
@@ -1846,7 +1846,7 @@
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>PRAMOD-JAIPUR</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
@@ -1900,7 +1900,7 @@
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>ANIL KUMAR PANDIT</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
@@ -1954,7 +1954,7 @@
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MANOJ TOMAR</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
@@ -2014,7 +2014,7 @@
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
@@ -2068,7 +2068,7 @@
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MANOJ TOMAR</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
@@ -2122,7 +2122,7 @@
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">
@@ -2182,7 +2182,7 @@
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H32" t="inlineStr">
@@ -2236,7 +2236,7 @@
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H33" t="inlineStr">
@@ -2290,7 +2290,7 @@
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H34" t="inlineStr">
@@ -2344,7 +2344,7 @@
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>SURESH</t>
         </is>
       </c>
       <c r="H35" t="inlineStr">
@@ -2398,7 +2398,7 @@
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MANOJ TOMAR</t>
         </is>
       </c>
       <c r="H36" t="inlineStr">
@@ -2452,7 +2452,7 @@
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MANOJ TOMAR</t>
         </is>
       </c>
       <c r="H37" t="inlineStr">
@@ -2506,7 +2506,7 @@
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H38" t="inlineStr">
@@ -2560,7 +2560,7 @@
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>ANIL KUMAR PANDIT</t>
         </is>
       </c>
       <c r="H39" t="inlineStr">
@@ -2614,7 +2614,7 @@
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H40" t="inlineStr">
@@ -2668,7 +2668,7 @@
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H41" t="inlineStr">
@@ -2728,7 +2728,7 @@
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H42" t="inlineStr">
@@ -2788,7 +2788,7 @@
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H43" t="inlineStr">
@@ -2844,7 +2844,7 @@
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MANOJ TOMAR</t>
         </is>
       </c>
       <c r="H44" t="inlineStr">
@@ -2898,7 +2898,7 @@
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H45" t="inlineStr">
@@ -2952,7 +2952,7 @@
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H46" t="inlineStr">
@@ -3012,7 +3012,7 @@
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H47" t="inlineStr">
@@ -3066,7 +3066,7 @@
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H48" t="inlineStr">
@@ -3120,7 +3120,7 @@
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H49" t="inlineStr">
@@ -3174,7 +3174,7 @@
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MANOJ TOMAR</t>
         </is>
       </c>
       <c r="H50" t="inlineStr">
@@ -3228,7 +3228,7 @@
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>PRAMOD-JAIPUR</t>
         </is>
       </c>
       <c r="H51" t="inlineStr">
@@ -3282,7 +3282,7 @@
       </c>
       <c r="G52" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H52" t="inlineStr">
@@ -3336,7 +3336,7 @@
       </c>
       <c r="G53" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>PRAMOD-JAIPUR</t>
         </is>
       </c>
       <c r="H53" t="inlineStr">
@@ -3396,7 +3396,7 @@
       </c>
       <c r="G54" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H54" t="inlineStr">
@@ -3450,7 +3450,7 @@
       </c>
       <c r="G55" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>PRAMOD-JAIPUR</t>
         </is>
       </c>
       <c r="H55" t="inlineStr">
@@ -3510,7 +3510,7 @@
       </c>
       <c r="G56" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H56" t="inlineStr">
@@ -3570,7 +3570,7 @@
       </c>
       <c r="G57" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H57" t="inlineStr">
@@ -3624,7 +3624,7 @@
       </c>
       <c r="G58" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H58" t="inlineStr">
@@ -3678,7 +3678,7 @@
       </c>
       <c r="G59" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H59" t="inlineStr">
@@ -3732,7 +3732,7 @@
       </c>
       <c r="G60" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H60" t="inlineStr">
@@ -3786,7 +3786,7 @@
       </c>
       <c r="G61" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>RAJENDER KUMAR VERMA</t>
         </is>
       </c>
       <c r="H61" t="inlineStr">
@@ -3840,7 +3840,7 @@
       </c>
       <c r="G62" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>GIRJESH KUMAR</t>
         </is>
       </c>
       <c r="H62" t="inlineStr">
@@ -3894,7 +3894,7 @@
       </c>
       <c r="G63" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H63" t="inlineStr">
@@ -3948,7 +3948,7 @@
       </c>
       <c r="G64" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>PRAMOD-JAIPUR</t>
         </is>
       </c>
       <c r="H64" t="inlineStr">
@@ -4002,7 +4002,7 @@
       </c>
       <c r="G65" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>PRAMOD-JAIPUR</t>
         </is>
       </c>
       <c r="H65" t="inlineStr">
@@ -4056,7 +4056,7 @@
       </c>
       <c r="G66" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>SUKHVINDER SINGH</t>
         </is>
       </c>
       <c r="H66" t="inlineStr">
@@ -4116,7 +4116,7 @@
       </c>
       <c r="G67" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H67" t="inlineStr">
@@ -4170,7 +4170,7 @@
       </c>
       <c r="G68" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H68" t="inlineStr">
@@ -4224,7 +4224,7 @@
       </c>
       <c r="G69" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>PRAMOD-JAIPUR</t>
         </is>
       </c>
       <c r="H69" t="inlineStr">
@@ -4278,7 +4278,7 @@
       </c>
       <c r="G70" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>PRAMOD-JAIPUR</t>
         </is>
       </c>
       <c r="H70" t="inlineStr">
@@ -4294,15 +4294,21 @@
       <c r="J70" t="n">
         <v>201102</v>
       </c>
-      <c r="K70" t="inlineStr"/>
+      <c r="K70" t="n">
+        <v>9750</v>
+      </c>
       <c r="L70" t="inlineStr">
         <is>
-          <t>FLOW</t>
-        </is>
-      </c>
-      <c r="M70" t="inlineStr"/>
+          <t>SB</t>
+        </is>
+      </c>
+      <c r="M70" t="inlineStr">
+        <is>
+          <t>8%</t>
+        </is>
+      </c>
       <c r="N70" t="n">
-        <v>0</v>
+        <v>780</v>
       </c>
     </row>
     <row r="71">
@@ -4332,7 +4338,7 @@
       </c>
       <c r="G71" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H71" t="inlineStr">
@@ -4386,7 +4392,7 @@
       </c>
       <c r="G72" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>PRAMOD-JAIPUR</t>
         </is>
       </c>
       <c r="H72" t="inlineStr">
@@ -4440,7 +4446,7 @@
       </c>
       <c r="G73" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H73" t="inlineStr">
@@ -4500,7 +4506,7 @@
       </c>
       <c r="G74" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>SHAKEEL</t>
         </is>
       </c>
       <c r="H74" t="inlineStr">
@@ -4554,7 +4560,7 @@
       </c>
       <c r="G75" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>PRAMOD-JAIPUR</t>
         </is>
       </c>
       <c r="H75" t="inlineStr">
@@ -4614,7 +4620,7 @@
       </c>
       <c r="G76" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H76" t="inlineStr">
@@ -4668,7 +4674,7 @@
       </c>
       <c r="G77" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H77" t="inlineStr">
@@ -4728,7 +4734,7 @@
       </c>
       <c r="G78" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MANOJ TOMAR</t>
         </is>
       </c>
       <c r="H78" t="inlineStr">
@@ -4782,7 +4788,7 @@
       </c>
       <c r="G79" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>PRAMOD-JAIPUR</t>
         </is>
       </c>
       <c r="H79" t="inlineStr">
@@ -4836,7 +4842,7 @@
       </c>
       <c r="G80" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>PRAMOD-JAIPUR</t>
         </is>
       </c>
       <c r="H80" t="inlineStr">
@@ -4890,7 +4896,7 @@
       </c>
       <c r="G81" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>ANIL KUMAR PANDIT</t>
         </is>
       </c>
       <c r="H81" t="inlineStr">
@@ -4944,7 +4950,7 @@
       </c>
       <c r="G82" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>SUBHASH CHAND</t>
         </is>
       </c>
       <c r="H82" t="inlineStr">
@@ -4998,7 +5004,7 @@
       </c>
       <c r="G83" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H83" t="inlineStr">
@@ -5052,7 +5058,7 @@
       </c>
       <c r="G84" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H84" t="inlineStr">
@@ -5106,7 +5112,7 @@
       </c>
       <c r="G85" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H85" t="inlineStr">
@@ -5166,7 +5172,7 @@
       </c>
       <c r="G86" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H86" t="inlineStr">
@@ -5226,7 +5232,7 @@
       </c>
       <c r="G87" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H87" t="inlineStr">
@@ -5280,7 +5286,7 @@
       </c>
       <c r="G88" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>SUKHVINDER SINGH</t>
         </is>
       </c>
       <c r="H88" t="inlineStr">
@@ -5334,7 +5340,7 @@
       </c>
       <c r="G89" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>PRAMOD-JAIPUR</t>
         </is>
       </c>
       <c r="H89" t="inlineStr">
@@ -5394,7 +5400,7 @@
       </c>
       <c r="G90" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H90" t="inlineStr">
@@ -5448,7 +5454,7 @@
       </c>
       <c r="G91" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MANOJ TOMAR</t>
         </is>
       </c>
       <c r="H91" t="inlineStr">
@@ -5508,7 +5514,7 @@
       </c>
       <c r="G92" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H92" t="inlineStr">
@@ -5562,7 +5568,7 @@
       </c>
       <c r="G93" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>PRAMOD-JAIPUR</t>
         </is>
       </c>
       <c r="H93" t="inlineStr">
@@ -5616,7 +5622,7 @@
       </c>
       <c r="G94" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>ANIL KUMAR PANDIT</t>
         </is>
       </c>
       <c r="H94" t="inlineStr">
@@ -5670,7 +5676,7 @@
       </c>
       <c r="G95" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H95" t="inlineStr">
@@ -5724,7 +5730,7 @@
       </c>
       <c r="G96" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>BEENESH</t>
         </is>
       </c>
       <c r="H96" t="inlineStr">
@@ -5778,7 +5784,7 @@
       </c>
       <c r="G97" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H97" t="inlineStr">
@@ -5834,7 +5840,7 @@
       </c>
       <c r="G98" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>ANIL KUMAR PANDIT</t>
         </is>
       </c>
       <c r="H98" t="inlineStr">
@@ -5888,7 +5894,7 @@
       </c>
       <c r="G99" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H99" t="inlineStr">
@@ -5942,7 +5948,7 @@
       </c>
       <c r="G100" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H100" t="inlineStr">
@@ -6002,7 +6008,7 @@
       </c>
       <c r="G101" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H101" t="inlineStr">
@@ -6062,7 +6068,7 @@
       </c>
       <c r="G102" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>PRAMOD-JAIPUR</t>
         </is>
       </c>
       <c r="H102" t="inlineStr">
@@ -6116,7 +6122,7 @@
       </c>
       <c r="G103" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>SURESH</t>
         </is>
       </c>
       <c r="H103" t="inlineStr">
@@ -6170,7 +6176,7 @@
       </c>
       <c r="G104" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>SUKHVINDER SINGH</t>
         </is>
       </c>
       <c r="H104" t="inlineStr">
@@ -6230,7 +6236,7 @@
       </c>
       <c r="G105" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MANOJ TOMAR</t>
         </is>
       </c>
       <c r="H105" t="inlineStr">
@@ -6284,7 +6290,7 @@
       </c>
       <c r="G106" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>BEENESH</t>
         </is>
       </c>
       <c r="H106" t="inlineStr">
@@ -6338,7 +6344,7 @@
       </c>
       <c r="G107" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H107" t="inlineStr">
@@ -6392,7 +6398,7 @@
       </c>
       <c r="G108" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H108" t="inlineStr">
@@ -6452,7 +6458,7 @@
       </c>
       <c r="G109" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H109" t="inlineStr">
@@ -6512,7 +6518,7 @@
       </c>
       <c r="G110" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>BEENESH</t>
         </is>
       </c>
       <c r="H110" t="inlineStr">
@@ -6572,7 +6578,7 @@
       </c>
       <c r="G111" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H111" t="inlineStr">
@@ -6632,7 +6638,7 @@
       </c>
       <c r="G112" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>BEENESH</t>
         </is>
       </c>
       <c r="H112" t="inlineStr">
@@ -6649,7 +6655,7 @@
         <v>122010</v>
       </c>
       <c r="K112" t="n">
-        <v>6792</v>
+        <v>15715</v>
       </c>
       <c r="L112" t="inlineStr">
         <is>
@@ -6662,7 +6668,7 @@
         </is>
       </c>
       <c r="N112" t="n">
-        <v>543.36</v>
+        <v>1257.2</v>
       </c>
     </row>
     <row r="113">
@@ -6692,7 +6698,7 @@
       </c>
       <c r="G113" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H113" t="inlineStr">
@@ -6752,7 +6758,7 @@
       </c>
       <c r="G114" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MANOJ TOMAR</t>
         </is>
       </c>
       <c r="H114" t="inlineStr">
@@ -6806,7 +6812,7 @@
       </c>
       <c r="G115" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>PRAMOD-JAIPUR</t>
         </is>
       </c>
       <c r="H115" t="inlineStr">
@@ -6866,7 +6872,7 @@
       </c>
       <c r="G116" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H116" t="inlineStr">
@@ -6920,7 +6926,7 @@
       </c>
       <c r="G117" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H117" t="inlineStr">
@@ -6974,7 +6980,7 @@
       </c>
       <c r="G118" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>PRAMOD-JAIPUR</t>
         </is>
       </c>
       <c r="H118" t="inlineStr">
@@ -7028,7 +7034,7 @@
       </c>
       <c r="G119" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H119" t="inlineStr">
@@ -7082,7 +7088,7 @@
       </c>
       <c r="G120" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>SUBHASH CHAND</t>
         </is>
       </c>
       <c r="H120" t="inlineStr">
@@ -7136,7 +7142,7 @@
       </c>
       <c r="G121" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H121" t="inlineStr">
@@ -7190,7 +7196,7 @@
       </c>
       <c r="G122" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>SUKHVINDER SINGH</t>
         </is>
       </c>
       <c r="H122" t="inlineStr">
@@ -7250,7 +7256,7 @@
       </c>
       <c r="G123" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>PRAMOD-JAIPUR</t>
         </is>
       </c>
       <c r="H123" t="inlineStr">
@@ -7304,7 +7310,7 @@
       </c>
       <c r="G124" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H124" t="inlineStr">
@@ -7358,7 +7364,7 @@
       </c>
       <c r="G125" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H125" t="inlineStr">
@@ -7412,7 +7418,7 @@
       </c>
       <c r="G126" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H126" t="inlineStr">
@@ -7466,7 +7472,7 @@
       </c>
       <c r="G127" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H127" t="inlineStr">
@@ -7520,7 +7526,7 @@
       </c>
       <c r="G128" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>ANIL KUMAR PANDIT</t>
         </is>
       </c>
       <c r="H128" t="inlineStr">
@@ -7580,7 +7586,7 @@
       </c>
       <c r="G129" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H129" t="inlineStr">
@@ -7640,7 +7646,7 @@
       </c>
       <c r="G130" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>SUBHASH CHAND</t>
         </is>
       </c>
       <c r="H130" t="inlineStr">
@@ -7694,7 +7700,7 @@
       </c>
       <c r="G131" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>BEENESH</t>
         </is>
       </c>
       <c r="H131" t="inlineStr">
@@ -7748,7 +7754,7 @@
       </c>
       <c r="G132" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H132" t="inlineStr">
@@ -7808,7 +7814,7 @@
       </c>
       <c r="G133" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H133" t="inlineStr">
@@ -7862,7 +7868,7 @@
       </c>
       <c r="G134" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MANOJ TOMAR</t>
         </is>
       </c>
       <c r="H134" t="inlineStr">
@@ -7916,7 +7922,7 @@
       </c>
       <c r="G135" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H135" t="inlineStr">
@@ -7970,7 +7976,7 @@
       </c>
       <c r="G136" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H136" t="inlineStr">
@@ -8024,7 +8030,7 @@
       </c>
       <c r="G137" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MANOJ TOMAR</t>
         </is>
       </c>
       <c r="H137" t="inlineStr">
@@ -8078,7 +8084,7 @@
       </c>
       <c r="G138" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H138" t="inlineStr">
@@ -8132,7 +8138,7 @@
       </c>
       <c r="G139" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H139" t="inlineStr">
@@ -8186,7 +8192,7 @@
       </c>
       <c r="G140" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MANOJ TOMAR</t>
         </is>
       </c>
       <c r="H140" t="inlineStr">
@@ -8240,7 +8246,7 @@
       </c>
       <c r="G141" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H141" t="inlineStr">
@@ -8294,7 +8300,7 @@
       </c>
       <c r="G142" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>SUBHASH CHAND</t>
         </is>
       </c>
       <c r="H142" t="inlineStr">
@@ -8348,7 +8354,7 @@
       </c>
       <c r="G143" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MANOJ TOMAR</t>
         </is>
       </c>
       <c r="H143" t="inlineStr">
@@ -8402,7 +8408,7 @@
       </c>
       <c r="G144" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H144" t="inlineStr">
@@ -8456,7 +8462,7 @@
       </c>
       <c r="G145" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H145" t="inlineStr">
@@ -8510,7 +8516,7 @@
       </c>
       <c r="G146" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MANOJ TOMAR</t>
         </is>
       </c>
       <c r="H146" t="inlineStr">
@@ -8564,7 +8570,7 @@
       </c>
       <c r="G147" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H147" t="inlineStr">
@@ -8618,7 +8624,7 @@
       </c>
       <c r="G148" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H148" t="inlineStr">
@@ -8672,7 +8678,7 @@
       </c>
       <c r="G149" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>PRAMOD-JAIPUR</t>
         </is>
       </c>
       <c r="H149" t="inlineStr">
@@ -8726,7 +8732,7 @@
       </c>
       <c r="G150" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H150" t="inlineStr">
@@ -8780,7 +8786,7 @@
       </c>
       <c r="G151" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H151" t="inlineStr">
@@ -8834,7 +8840,7 @@
       </c>
       <c r="G152" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>PRAMOD-JAIPUR</t>
         </is>
       </c>
       <c r="H152" t="inlineStr">
@@ -8888,7 +8894,7 @@
       </c>
       <c r="G153" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>PRAMOD-JAIPUR</t>
         </is>
       </c>
       <c r="H153" t="inlineStr">
@@ -8942,7 +8948,7 @@
       </c>
       <c r="G154" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H154" t="inlineStr">
@@ -8996,7 +9002,7 @@
       </c>
       <c r="G155" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H155" t="inlineStr">
@@ -9050,7 +9056,7 @@
       </c>
       <c r="G156" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H156" t="inlineStr">
@@ -9104,7 +9110,7 @@
       </c>
       <c r="G157" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>ARVIND KUMAR</t>
         </is>
       </c>
       <c r="H157" t="inlineStr">
@@ -9164,7 +9170,7 @@
       </c>
       <c r="G158" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>BEENESH</t>
         </is>
       </c>
       <c r="H158" t="inlineStr">
@@ -9218,7 +9224,7 @@
       </c>
       <c r="G159" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H159" t="inlineStr">
@@ -9278,7 +9284,7 @@
       </c>
       <c r="G160" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H160" t="inlineStr">
@@ -9332,7 +9338,7 @@
       </c>
       <c r="G161" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H161" t="inlineStr">
@@ -9386,7 +9392,7 @@
       </c>
       <c r="G162" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H162" t="inlineStr">
@@ -9440,7 +9446,7 @@
       </c>
       <c r="G163" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>PRAMOD-JAIPUR</t>
         </is>
       </c>
       <c r="H163" t="inlineStr">
@@ -9494,7 +9500,7 @@
       </c>
       <c r="G164" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>SHAKEEL</t>
         </is>
       </c>
       <c r="H164" t="inlineStr">
@@ -9548,7 +9554,7 @@
       </c>
       <c r="G165" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>GURPREET SINGH</t>
         </is>
       </c>
       <c r="H165" t="inlineStr">
@@ -9602,7 +9608,7 @@
       </c>
       <c r="G166" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>PRAMOD-JAIPUR</t>
         </is>
       </c>
       <c r="H166" t="inlineStr">
@@ -9662,7 +9668,7 @@
       </c>
       <c r="G167" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H167" t="inlineStr">
@@ -9718,7 +9724,7 @@
       </c>
       <c r="G168" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H168" t="inlineStr">
@@ -9772,7 +9778,7 @@
       </c>
       <c r="G169" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H169" t="inlineStr">
@@ -9826,7 +9832,7 @@
       </c>
       <c r="G170" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H170" t="inlineStr">
@@ -9886,7 +9892,7 @@
       </c>
       <c r="G171" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H171" t="inlineStr">
@@ -9940,7 +9946,7 @@
       </c>
       <c r="G172" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>SHAKEEL</t>
         </is>
       </c>
       <c r="H172" t="inlineStr">
@@ -9957,7 +9963,7 @@
         <v>201301</v>
       </c>
       <c r="K172" t="n">
-        <v>3480</v>
+        <v>4380</v>
       </c>
       <c r="L172" t="inlineStr">
         <is>
@@ -9970,7 +9976,7 @@
         </is>
       </c>
       <c r="N172" t="n">
-        <v>278.4</v>
+        <v>350.4</v>
       </c>
     </row>
     <row r="173">
@@ -10000,7 +10006,7 @@
       </c>
       <c r="G173" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>SHAKEEL</t>
         </is>
       </c>
       <c r="H173" t="inlineStr">
@@ -10054,7 +10060,7 @@
       </c>
       <c r="G174" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>ANIL KUMAR PANDIT</t>
         </is>
       </c>
       <c r="H174" t="inlineStr">
@@ -10108,7 +10114,7 @@
       </c>
       <c r="G175" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MANOJ TOMAR</t>
         </is>
       </c>
       <c r="H175" t="inlineStr">
@@ -10162,7 +10168,7 @@
       </c>
       <c r="G176" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>PRAMOD-JAIPUR</t>
         </is>
       </c>
       <c r="H176" t="inlineStr">
@@ -10216,7 +10222,7 @@
       </c>
       <c r="G177" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H177" t="inlineStr">
@@ -10270,7 +10276,7 @@
       </c>
       <c r="G178" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>RAJENDER KUMAR VERMA</t>
         </is>
       </c>
       <c r="H178" t="inlineStr">
@@ -10330,7 +10336,7 @@
       </c>
       <c r="G179" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MANOJ TOMAR</t>
         </is>
       </c>
       <c r="H179" t="inlineStr">
@@ -10384,7 +10390,7 @@
       </c>
       <c r="G180" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H180" t="inlineStr">
@@ -10444,7 +10450,7 @@
       </c>
       <c r="G181" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H181" t="inlineStr">
@@ -10498,7 +10504,7 @@
       </c>
       <c r="G182" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>ANIL KUMAR PANDIT</t>
         </is>
       </c>
       <c r="H182" t="inlineStr">
@@ -10552,7 +10558,7 @@
       </c>
       <c r="G183" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H183" t="inlineStr">
@@ -10606,7 +10612,7 @@
       </c>
       <c r="G184" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H184" t="inlineStr">
@@ -10660,7 +10666,7 @@
       </c>
       <c r="G185" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H185" t="inlineStr">
@@ -10714,7 +10720,7 @@
       </c>
       <c r="G186" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>SUKHVINDER SINGH</t>
         </is>
       </c>
       <c r="H186" t="inlineStr">
@@ -10768,7 +10774,7 @@
       </c>
       <c r="G187" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H187" t="inlineStr">
@@ -10822,7 +10828,7 @@
       </c>
       <c r="G188" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H188" t="inlineStr">
@@ -10876,7 +10882,7 @@
       </c>
       <c r="G189" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>SUBHASH CHAND</t>
         </is>
       </c>
       <c r="H189" t="inlineStr">
@@ -10936,7 +10942,7 @@
       </c>
       <c r="G190" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>PRAMOD-JAIPUR</t>
         </is>
       </c>
       <c r="H190" t="inlineStr">
@@ -10996,7 +11002,7 @@
       </c>
       <c r="G191" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H191" t="inlineStr">
@@ -11056,7 +11062,7 @@
       </c>
       <c r="G192" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H192" t="inlineStr">
@@ -11110,7 +11116,7 @@
       </c>
       <c r="G193" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H193" t="inlineStr">
@@ -11170,7 +11176,7 @@
       </c>
       <c r="G194" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H194" t="inlineStr">
@@ -11224,7 +11230,7 @@
       </c>
       <c r="G195" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H195" t="inlineStr">
@@ -11278,7 +11284,7 @@
       </c>
       <c r="G196" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H196" t="inlineStr">
@@ -11338,7 +11344,7 @@
       </c>
       <c r="G197" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>ARVIND KUMAR</t>
         </is>
       </c>
       <c r="H197" t="inlineStr">
@@ -11392,7 +11398,7 @@
       </c>
       <c r="G198" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>BEENESH</t>
         </is>
       </c>
       <c r="H198" t="inlineStr">
@@ -11446,7 +11452,7 @@
       </c>
       <c r="G199" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H199" t="inlineStr">
@@ -11500,7 +11506,7 @@
       </c>
       <c r="G200" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>PRAMOD-JAIPUR</t>
         </is>
       </c>
       <c r="H200" t="inlineStr">
@@ -11554,7 +11560,7 @@
       </c>
       <c r="G201" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>PRAMOD-JAIPUR</t>
         </is>
       </c>
       <c r="H201" t="inlineStr">
@@ -11614,7 +11620,7 @@
       </c>
       <c r="G202" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H202" t="inlineStr">
@@ -11668,7 +11674,7 @@
       </c>
       <c r="G203" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>BEENESH</t>
         </is>
       </c>
       <c r="H203" t="inlineStr">
@@ -11722,7 +11728,7 @@
       </c>
       <c r="G204" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>PRAMOD-JAIPUR</t>
         </is>
       </c>
       <c r="H204" t="inlineStr">
@@ -11782,7 +11788,7 @@
       </c>
       <c r="G205" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H205" t="inlineStr">
@@ -11836,7 +11842,7 @@
       </c>
       <c r="G206" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H206" t="inlineStr">
@@ -11890,7 +11896,7 @@
       </c>
       <c r="G207" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H207" t="inlineStr">
@@ -11944,7 +11950,7 @@
       </c>
       <c r="G208" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>PRAMOD-JAIPUR</t>
         </is>
       </c>
       <c r="H208" t="inlineStr">
@@ -11998,7 +12004,7 @@
       </c>
       <c r="G209" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H209" t="inlineStr">
@@ -12052,7 +12058,7 @@
       </c>
       <c r="G210" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H210" t="inlineStr">
@@ -12112,7 +12118,7 @@
       </c>
       <c r="G211" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>PRAMOD-JAIPUR</t>
         </is>
       </c>
       <c r="H211" t="inlineStr">
@@ -12166,7 +12172,7 @@
       </c>
       <c r="G212" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H212" t="inlineStr">
@@ -12226,7 +12232,7 @@
       </c>
       <c r="G213" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H213" t="inlineStr">
@@ -12280,7 +12286,7 @@
       </c>
       <c r="G214" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H214" t="inlineStr">
@@ -12334,7 +12340,7 @@
       </c>
       <c r="G215" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H215" t="inlineStr">
@@ -12394,7 +12400,7 @@
       </c>
       <c r="G216" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H216" t="inlineStr">
@@ -12411,16 +12417,20 @@
         <v>110008</v>
       </c>
       <c r="K216" t="n">
-        <v>31481</v>
+        <v>36598</v>
       </c>
       <c r="L216" t="inlineStr">
         <is>
-          <t>PART PAID</t>
-        </is>
-      </c>
-      <c r="M216" t="inlineStr"/>
+          <t>NM</t>
+        </is>
+      </c>
+      <c r="M216" t="inlineStr">
+        <is>
+          <t>7%</t>
+        </is>
+      </c>
       <c r="N216" t="n">
-        <v>0</v>
+        <v>2561.86</v>
       </c>
     </row>
     <row r="217">
@@ -12450,7 +12460,7 @@
       </c>
       <c r="G217" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H217" t="inlineStr">
@@ -12504,7 +12514,7 @@
       </c>
       <c r="G218" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>BEENESH</t>
         </is>
       </c>
       <c r="H218" t="inlineStr">
@@ -12564,7 +12574,7 @@
       </c>
       <c r="G219" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H219" t="inlineStr">
@@ -12618,7 +12628,7 @@
       </c>
       <c r="G220" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H220" t="inlineStr">
@@ -12678,7 +12688,7 @@
       </c>
       <c r="G221" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H221" t="inlineStr">
@@ -12732,7 +12742,7 @@
       </c>
       <c r="G222" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H222" t="inlineStr">
@@ -12786,7 +12796,7 @@
       </c>
       <c r="G223" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H223" t="inlineStr">
@@ -12846,7 +12856,7 @@
       </c>
       <c r="G224" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>SURESH</t>
         </is>
       </c>
       <c r="H224" t="inlineStr">
@@ -12900,7 +12910,7 @@
       </c>
       <c r="G225" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H225" t="inlineStr">
@@ -12960,7 +12970,7 @@
       </c>
       <c r="G226" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H226" t="inlineStr">
@@ -13014,7 +13024,7 @@
       </c>
       <c r="G227" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>PRAMOD-JAIPUR</t>
         </is>
       </c>
       <c r="H227" t="inlineStr">
@@ -13068,7 +13078,7 @@
       </c>
       <c r="G228" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H228" t="inlineStr">
@@ -13122,7 +13132,7 @@
       </c>
       <c r="G229" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>PRAMOD-JAIPUR</t>
         </is>
       </c>
       <c r="H229" t="inlineStr">
@@ -13182,7 +13192,7 @@
       </c>
       <c r="G230" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>PRAMOD-JAIPUR</t>
         </is>
       </c>
       <c r="H230" t="inlineStr">
@@ -13242,7 +13252,7 @@
       </c>
       <c r="G231" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H231" t="inlineStr">
@@ -13296,7 +13306,7 @@
       </c>
       <c r="G232" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>GURPREET SINGH</t>
         </is>
       </c>
       <c r="H232" t="inlineStr">
@@ -13350,7 +13360,7 @@
       </c>
       <c r="G233" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H233" t="inlineStr">
@@ -13404,7 +13414,7 @@
       </c>
       <c r="G234" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H234" t="inlineStr">
@@ -13464,7 +13474,7 @@
       </c>
       <c r="G235" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>SURESH</t>
         </is>
       </c>
       <c r="H235" t="inlineStr">
@@ -13518,7 +13528,7 @@
       </c>
       <c r="G236" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H236" t="inlineStr">
@@ -13572,7 +13582,7 @@
       </c>
       <c r="G237" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>PRAMOD-JAIPUR</t>
         </is>
       </c>
       <c r="H237" t="inlineStr">
@@ -13626,7 +13636,7 @@
       </c>
       <c r="G238" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MANOJ TOMAR</t>
         </is>
       </c>
       <c r="H238" t="inlineStr">
@@ -13680,7 +13690,7 @@
       </c>
       <c r="G239" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H239" t="inlineStr">
@@ -13734,7 +13744,7 @@
       </c>
       <c r="G240" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H240" t="inlineStr">
@@ -13750,15 +13760,21 @@
       <c r="J240" t="n">
         <v>335051</v>
       </c>
-      <c r="K240" t="inlineStr"/>
+      <c r="K240" t="n">
+        <v>32758</v>
+      </c>
       <c r="L240" t="inlineStr">
         <is>
-          <t>FLOW</t>
-        </is>
-      </c>
-      <c r="M240" t="inlineStr"/>
+          <t>SB</t>
+        </is>
+      </c>
+      <c r="M240" t="inlineStr">
+        <is>
+          <t>8%</t>
+        </is>
+      </c>
       <c r="N240" t="n">
-        <v>0</v>
+        <v>2620.64</v>
       </c>
     </row>
     <row r="241">
@@ -13788,7 +13804,7 @@
       </c>
       <c r="G241" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>PRAMOD-JAIPUR</t>
         </is>
       </c>
       <c r="H241" t="inlineStr">
@@ -13842,7 +13858,7 @@
       </c>
       <c r="G242" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H242" t="inlineStr">
@@ -13896,7 +13912,7 @@
       </c>
       <c r="G243" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>SUBHASH CHAND</t>
         </is>
       </c>
       <c r="H243" t="inlineStr">
@@ -13950,7 +13966,7 @@
       </c>
       <c r="G244" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H244" t="inlineStr">
@@ -13966,15 +13982,21 @@
       <c r="J244" t="n">
         <v>222125</v>
       </c>
-      <c r="K244" t="inlineStr"/>
+      <c r="K244" t="n">
+        <v>4981</v>
+      </c>
       <c r="L244" t="inlineStr">
         <is>
-          <t>FLOW</t>
-        </is>
-      </c>
-      <c r="M244" t="inlineStr"/>
+          <t>SB</t>
+        </is>
+      </c>
+      <c r="M244" t="inlineStr">
+        <is>
+          <t>8%</t>
+        </is>
+      </c>
       <c r="N244" t="n">
-        <v>0</v>
+        <v>398.48</v>
       </c>
     </row>
     <row r="245">
@@ -14004,7 +14026,7 @@
       </c>
       <c r="G245" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H245" t="inlineStr">
@@ -14064,7 +14086,7 @@
       </c>
       <c r="G246" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>BEENESH</t>
         </is>
       </c>
       <c r="H246" t="inlineStr">
@@ -14118,7 +14140,7 @@
       </c>
       <c r="G247" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>BEENESH</t>
         </is>
       </c>
       <c r="H247" t="inlineStr">
@@ -14135,7 +14157,7 @@
         <v>122009</v>
       </c>
       <c r="K247" t="n">
-        <v>9143</v>
+        <v>20209</v>
       </c>
       <c r="L247" t="inlineStr">
         <is>
@@ -14148,7 +14170,7 @@
         </is>
       </c>
       <c r="N247" t="n">
-        <v>731.4400000000001</v>
+        <v>1616.72</v>
       </c>
     </row>
     <row r="248">
@@ -14178,7 +14200,7 @@
       </c>
       <c r="G248" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H248" t="inlineStr">
@@ -14238,7 +14260,7 @@
       </c>
       <c r="G249" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H249" t="inlineStr">
@@ -14292,7 +14314,7 @@
       </c>
       <c r="G250" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H250" t="inlineStr">
@@ -14346,7 +14368,7 @@
       </c>
       <c r="G251" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H251" t="inlineStr">
@@ -14400,7 +14422,7 @@
       </c>
       <c r="G252" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>BEENESH</t>
         </is>
       </c>
       <c r="H252" t="inlineStr">
@@ -14454,7 +14476,7 @@
       </c>
       <c r="G253" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>SUKHVINDER SINGH</t>
         </is>
       </c>
       <c r="H253" t="inlineStr">
@@ -14508,7 +14530,7 @@
       </c>
       <c r="G254" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>PRAMOD-JAIPUR</t>
         </is>
       </c>
       <c r="H254" t="inlineStr">
@@ -14568,7 +14590,7 @@
       </c>
       <c r="G255" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H255" t="inlineStr">
@@ -14622,7 +14644,7 @@
       </c>
       <c r="G256" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H256" t="inlineStr">
@@ -14676,7 +14698,7 @@
       </c>
       <c r="G257" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H257" t="inlineStr">
@@ -14730,7 +14752,7 @@
       </c>
       <c r="G258" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H258" t="inlineStr">
@@ -14784,7 +14806,7 @@
       </c>
       <c r="G259" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>SUKHVINDER SINGH</t>
         </is>
       </c>
       <c r="H259" t="inlineStr">
@@ -14838,7 +14860,7 @@
       </c>
       <c r="G260" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>ARVIND KUMAR</t>
         </is>
       </c>
       <c r="H260" t="inlineStr">
@@ -14892,7 +14914,7 @@
       </c>
       <c r="G261" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>PRAMOD-JAIPUR</t>
         </is>
       </c>
       <c r="H261" t="inlineStr">
@@ -14952,7 +14974,7 @@
       </c>
       <c r="G262" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H262" t="inlineStr">
@@ -15012,7 +15034,7 @@
       </c>
       <c r="G263" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>PRAMOD-JAIPUR</t>
         </is>
       </c>
       <c r="H263" t="inlineStr">
@@ -15072,7 +15094,7 @@
       </c>
       <c r="G264" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>PRAMOD-JAIPUR</t>
         </is>
       </c>
       <c r="H264" t="inlineStr">
@@ -15126,7 +15148,7 @@
       </c>
       <c r="G265" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H265" t="inlineStr">
@@ -15186,7 +15208,7 @@
       </c>
       <c r="G266" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H266" t="inlineStr">
@@ -15246,7 +15268,7 @@
       </c>
       <c r="G267" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H267" t="inlineStr">
@@ -15300,7 +15322,7 @@
       </c>
       <c r="G268" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>PRAMOD-JAIPUR</t>
         </is>
       </c>
       <c r="H268" t="inlineStr">
@@ -15360,7 +15382,7 @@
       </c>
       <c r="G269" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H269" t="inlineStr">
@@ -15420,7 +15442,7 @@
       </c>
       <c r="G270" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>PRAMOD-JAIPUR</t>
         </is>
       </c>
       <c r="H270" t="inlineStr">
@@ -15480,7 +15502,7 @@
       </c>
       <c r="G271" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H271" t="inlineStr">
@@ -15540,7 +15562,7 @@
       </c>
       <c r="G272" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>GURPREET SINGH</t>
         </is>
       </c>
       <c r="H272" t="inlineStr">
@@ -15594,7 +15616,7 @@
       </c>
       <c r="G273" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H273" t="inlineStr">
@@ -15648,7 +15670,7 @@
       </c>
       <c r="G274" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H274" t="inlineStr">
@@ -15702,7 +15724,7 @@
       </c>
       <c r="G275" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>PRAMOD-JAIPUR</t>
         </is>
       </c>
       <c r="H275" t="inlineStr">
@@ -15756,7 +15778,7 @@
       </c>
       <c r="G276" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>ANIL KUMAR PANDIT</t>
         </is>
       </c>
       <c r="H276" t="inlineStr">
@@ -15810,7 +15832,7 @@
       </c>
       <c r="G277" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H277" t="inlineStr">
@@ -15870,7 +15892,7 @@
       </c>
       <c r="G278" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H278" t="inlineStr">
@@ -15924,7 +15946,7 @@
       </c>
       <c r="G279" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H279" t="inlineStr">
@@ -15978,7 +16000,7 @@
       </c>
       <c r="G280" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>PRAMOD-JAIPUR</t>
         </is>
       </c>
       <c r="H280" t="inlineStr">
@@ -16032,7 +16054,7 @@
       </c>
       <c r="G281" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H281" t="inlineStr">
@@ -16086,7 +16108,7 @@
       </c>
       <c r="G282" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>PRAMOD-JAIPUR</t>
         </is>
       </c>
       <c r="H282" t="inlineStr">
@@ -16140,7 +16162,7 @@
       </c>
       <c r="G283" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H283" t="inlineStr">
@@ -16200,7 +16222,7 @@
       </c>
       <c r="G284" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H284" t="inlineStr">
@@ -16260,7 +16282,7 @@
       </c>
       <c r="G285" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>PRAMOD-JAIPUR</t>
         </is>
       </c>
       <c r="H285" t="inlineStr">
@@ -16314,7 +16336,7 @@
       </c>
       <c r="G286" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>PRAMOD-JAIPUR</t>
         </is>
       </c>
       <c r="H286" t="inlineStr">
@@ -16368,7 +16390,7 @@
       </c>
       <c r="G287" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MANOJ TOMAR</t>
         </is>
       </c>
       <c r="H287" t="inlineStr">
@@ -16422,7 +16444,7 @@
       </c>
       <c r="G288" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H288" t="inlineStr">
@@ -16482,7 +16504,7 @@
       </c>
       <c r="G289" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H289" t="inlineStr">
@@ -16542,7 +16564,7 @@
       </c>
       <c r="G290" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H290" t="inlineStr">
@@ -16596,7 +16618,7 @@
       </c>
       <c r="G291" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>SUBHASH CHAND</t>
         </is>
       </c>
       <c r="H291" t="inlineStr">
@@ -16613,7 +16635,7 @@
         <v>201102</v>
       </c>
       <c r="K291" t="n">
-        <v>4378</v>
+        <v>19541</v>
       </c>
       <c r="L291" t="inlineStr">
         <is>
@@ -16626,7 +16648,7 @@
         </is>
       </c>
       <c r="N291" t="n">
-        <v>350.24</v>
+        <v>1563.28</v>
       </c>
     </row>
     <row r="292">
@@ -16656,7 +16678,7 @@
       </c>
       <c r="G292" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H292" t="inlineStr">
@@ -16716,7 +16738,7 @@
       </c>
       <c r="G293" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>PRAMOD-JAIPUR</t>
         </is>
       </c>
       <c r="H293" t="inlineStr">
@@ -16776,7 +16798,7 @@
       </c>
       <c r="G294" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H294" t="inlineStr">
@@ -16836,7 +16858,7 @@
       </c>
       <c r="G295" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H295" t="inlineStr">
@@ -16890,7 +16912,7 @@
       </c>
       <c r="G296" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H296" t="inlineStr">
@@ -16944,7 +16966,7 @@
       </c>
       <c r="G297" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H297" t="inlineStr">
@@ -16998,7 +17020,7 @@
       </c>
       <c r="G298" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>PRAMOD-JAIPUR</t>
         </is>
       </c>
       <c r="H298" t="inlineStr">
@@ -17052,7 +17074,7 @@
       </c>
       <c r="G299" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H299" t="inlineStr">
@@ -17106,7 +17128,7 @@
       </c>
       <c r="G300" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>BEENESH</t>
         </is>
       </c>
       <c r="H300" t="inlineStr">
@@ -17160,7 +17182,7 @@
       </c>
       <c r="G301" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H301" t="inlineStr">
@@ -17220,7 +17242,7 @@
       </c>
       <c r="G302" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H302" t="inlineStr">
@@ -17274,7 +17296,7 @@
       </c>
       <c r="G303" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>PRAMOD-JAIPUR</t>
         </is>
       </c>
       <c r="H303" t="inlineStr">
@@ -17328,7 +17350,7 @@
       </c>
       <c r="G304" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>GIRJESH KUMAR</t>
         </is>
       </c>
       <c r="H304" t="inlineStr">
@@ -17388,7 +17410,7 @@
       </c>
       <c r="G305" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H305" t="inlineStr">
@@ -17442,7 +17464,7 @@
       </c>
       <c r="G306" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H306" t="inlineStr">
@@ -17496,7 +17518,7 @@
       </c>
       <c r="G307" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H307" t="inlineStr">
@@ -17550,7 +17572,7 @@
       </c>
       <c r="G308" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H308" t="inlineStr">
@@ -17604,7 +17626,7 @@
       </c>
       <c r="G309" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>BEENESH</t>
         </is>
       </c>
       <c r="H309" t="inlineStr">
@@ -17658,7 +17680,7 @@
       </c>
       <c r="G310" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H310" t="inlineStr">
@@ -17712,7 +17734,7 @@
       </c>
       <c r="G311" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>SUBHASH CHAND</t>
         </is>
       </c>
       <c r="H311" t="inlineStr">
@@ -17766,7 +17788,7 @@
       </c>
       <c r="G312" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H312" t="inlineStr">
@@ -17820,7 +17842,7 @@
       </c>
       <c r="G313" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>ANIL KUMAR PANDIT</t>
         </is>
       </c>
       <c r="H313" t="inlineStr">
@@ -17836,15 +17858,21 @@
       <c r="J313" t="n">
         <v>110091</v>
       </c>
-      <c r="K313" t="inlineStr"/>
+      <c r="K313" t="n">
+        <v>4378</v>
+      </c>
       <c r="L313" t="inlineStr">
         <is>
-          <t>FLOW</t>
-        </is>
-      </c>
-      <c r="M313" t="inlineStr"/>
+          <t>SB</t>
+        </is>
+      </c>
+      <c r="M313" t="inlineStr">
+        <is>
+          <t>8%</t>
+        </is>
+      </c>
       <c r="N313" t="n">
-        <v>0</v>
+        <v>350.24</v>
       </c>
     </row>
     <row r="314">
@@ -17874,7 +17902,7 @@
       </c>
       <c r="G314" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H314" t="inlineStr">
@@ -17928,7 +17956,7 @@
       </c>
       <c r="G315" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>PRAMOD-JAIPUR</t>
         </is>
       </c>
       <c r="H315" t="inlineStr">
@@ -17982,7 +18010,7 @@
       </c>
       <c r="G316" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H316" t="inlineStr">
@@ -18036,7 +18064,7 @@
       </c>
       <c r="G317" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>PRAMOD-JAIPUR</t>
         </is>
       </c>
       <c r="H317" t="inlineStr">
@@ -18090,7 +18118,7 @@
       </c>
       <c r="G318" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H318" t="inlineStr">
@@ -18150,7 +18178,7 @@
       </c>
       <c r="G319" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>PRAMOD-JAIPUR</t>
         </is>
       </c>
       <c r="H319" t="inlineStr">
@@ -18204,7 +18232,7 @@
       </c>
       <c r="G320" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H320" t="inlineStr">
@@ -18258,7 +18286,7 @@
       </c>
       <c r="G321" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H321" t="inlineStr">
@@ -18312,7 +18340,7 @@
       </c>
       <c r="G322" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H322" t="inlineStr">
@@ -18372,7 +18400,7 @@
       </c>
       <c r="G323" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H323" t="inlineStr">
@@ -18432,7 +18460,7 @@
       </c>
       <c r="G324" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>ANIL KUMAR PANDIT</t>
         </is>
       </c>
       <c r="H324" t="inlineStr">
@@ -18486,7 +18514,7 @@
       </c>
       <c r="G325" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H325" t="inlineStr">
@@ -18540,7 +18568,7 @@
       </c>
       <c r="G326" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>SURESH</t>
         </is>
       </c>
       <c r="H326" t="inlineStr">
@@ -18594,7 +18622,7 @@
       </c>
       <c r="G327" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H327" t="inlineStr">
@@ -18648,7 +18676,7 @@
       </c>
       <c r="G328" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H328" t="inlineStr">
@@ -18702,7 +18730,7 @@
       </c>
       <c r="G329" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H329" t="inlineStr">
@@ -18762,7 +18790,7 @@
       </c>
       <c r="G330" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H330" t="inlineStr">
@@ -18822,7 +18850,7 @@
       </c>
       <c r="G331" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H331" t="inlineStr">
@@ -18876,7 +18904,7 @@
       </c>
       <c r="G332" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>BEENESH</t>
         </is>
       </c>
       <c r="H332" t="inlineStr">
@@ -18930,7 +18958,7 @@
       </c>
       <c r="G333" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H333" t="inlineStr">
@@ -18984,7 +19012,7 @@
       </c>
       <c r="G334" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H334" t="inlineStr">
@@ -19044,7 +19072,7 @@
       </c>
       <c r="G335" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H335" t="inlineStr">
@@ -19098,7 +19126,7 @@
       </c>
       <c r="G336" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>RAJENDER KUMAR VERMA</t>
         </is>
       </c>
       <c r="H336" t="inlineStr">
@@ -19152,7 +19180,7 @@
       </c>
       <c r="G337" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H337" t="inlineStr">
@@ -19206,7 +19234,7 @@
       </c>
       <c r="G338" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H338" t="inlineStr">
@@ -19260,7 +19288,7 @@
       </c>
       <c r="G339" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>PRAMOD-JAIPUR</t>
         </is>
       </c>
       <c r="H339" t="inlineStr">
@@ -19314,7 +19342,7 @@
       </c>
       <c r="G340" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H340" t="inlineStr">
@@ -19330,15 +19358,21 @@
       <c r="J340" t="n">
         <v>342005</v>
       </c>
-      <c r="K340" t="inlineStr"/>
+      <c r="K340" t="n">
+        <v>16183</v>
+      </c>
       <c r="L340" t="inlineStr">
         <is>
-          <t>FLOW</t>
-        </is>
-      </c>
-      <c r="M340" t="inlineStr"/>
+          <t>SB</t>
+        </is>
+      </c>
+      <c r="M340" t="inlineStr">
+        <is>
+          <t>8%</t>
+        </is>
+      </c>
       <c r="N340" t="n">
-        <v>0</v>
+        <v>1294.64</v>
       </c>
     </row>
     <row r="341">
@@ -19368,7 +19402,7 @@
       </c>
       <c r="G341" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H341" t="inlineStr">
@@ -19422,7 +19456,7 @@
       </c>
       <c r="G342" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>PRAMOD-JAIPUR</t>
         </is>
       </c>
       <c r="H342" t="inlineStr">
@@ -19476,7 +19510,7 @@
       </c>
       <c r="G343" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>ANIL KUMAR PANDIT</t>
         </is>
       </c>
       <c r="H343" t="inlineStr">
@@ -19530,7 +19564,7 @@
       </c>
       <c r="G344" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H344" t="inlineStr">
@@ -19584,7 +19618,7 @@
       </c>
       <c r="G345" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H345" t="inlineStr">
@@ -19644,7 +19678,7 @@
       </c>
       <c r="G346" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>RAJENDER KUMAR VERMA</t>
         </is>
       </c>
       <c r="H346" t="inlineStr">
@@ -19698,7 +19732,7 @@
       </c>
       <c r="G347" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H347" t="inlineStr">
@@ -19758,7 +19792,7 @@
       </c>
       <c r="G348" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>SURESH</t>
         </is>
       </c>
       <c r="H348" t="inlineStr">
@@ -19812,7 +19846,7 @@
       </c>
       <c r="G349" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H349" t="inlineStr">
@@ -19866,7 +19900,7 @@
       </c>
       <c r="G350" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H350" t="inlineStr">
@@ -19920,7 +19954,7 @@
       </c>
       <c r="G351" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>PRAMOD-JAIPUR</t>
         </is>
       </c>
       <c r="H351" t="inlineStr">
@@ -19974,7 +20008,7 @@
       </c>
       <c r="G352" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>BEENESH</t>
         </is>
       </c>
       <c r="H352" t="inlineStr">
@@ -20034,7 +20068,7 @@
       </c>
       <c r="G353" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H353" t="inlineStr">
@@ -20094,7 +20128,7 @@
       </c>
       <c r="G354" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>PRAMOD-JAIPUR</t>
         </is>
       </c>
       <c r="H354" t="inlineStr">
@@ -20148,7 +20182,7 @@
       </c>
       <c r="G355" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H355" t="inlineStr">
@@ -20208,7 +20242,7 @@
       </c>
       <c r="G356" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>SHAKEEL</t>
         </is>
       </c>
       <c r="H356" t="inlineStr">
@@ -20262,7 +20296,7 @@
       </c>
       <c r="G357" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H357" t="inlineStr">
@@ -20322,7 +20356,7 @@
       </c>
       <c r="G358" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H358" t="inlineStr">
@@ -20382,7 +20416,7 @@
       </c>
       <c r="G359" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>PRAMOD-JAIPUR</t>
         </is>
       </c>
       <c r="H359" t="inlineStr">
@@ -20436,7 +20470,7 @@
       </c>
       <c r="G360" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H360" t="inlineStr">
@@ -20453,7 +20487,7 @@
         <v>110019</v>
       </c>
       <c r="K360" t="n">
-        <v>8138</v>
+        <v>9202</v>
       </c>
       <c r="L360" t="inlineStr">
         <is>
@@ -20466,7 +20500,7 @@
         </is>
       </c>
       <c r="N360" t="n">
-        <v>651.04</v>
+        <v>736.16</v>
       </c>
     </row>
     <row r="361">
@@ -20496,7 +20530,7 @@
       </c>
       <c r="G361" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H361" t="inlineStr">
@@ -20550,7 +20584,7 @@
       </c>
       <c r="G362" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H362" t="inlineStr">
@@ -20604,7 +20638,7 @@
       </c>
       <c r="G363" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H363" t="inlineStr">
@@ -20664,7 +20698,7 @@
       </c>
       <c r="G364" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H364" t="inlineStr">
@@ -20718,7 +20752,7 @@
       </c>
       <c r="G365" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H365" t="inlineStr">
@@ -20772,7 +20806,7 @@
       </c>
       <c r="G366" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>PRAMOD-JAIPUR</t>
         </is>
       </c>
       <c r="H366" t="inlineStr">
@@ -20826,7 +20860,7 @@
       </c>
       <c r="G367" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>ANIL KUMAR PANDIT</t>
         </is>
       </c>
       <c r="H367" t="inlineStr">
@@ -20880,7 +20914,7 @@
       </c>
       <c r="G368" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>PRAMOD-JAIPUR</t>
         </is>
       </c>
       <c r="H368" t="inlineStr">
@@ -20934,7 +20968,7 @@
       </c>
       <c r="G369" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H369" t="inlineStr">
@@ -20988,7 +21022,7 @@
       </c>
       <c r="G370" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>SHAKEEL</t>
         </is>
       </c>
       <c r="H370" t="inlineStr">
@@ -21042,7 +21076,7 @@
       </c>
       <c r="G371" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>PRAMOD-JAIPUR</t>
         </is>
       </c>
       <c r="H371" t="inlineStr">
@@ -21102,7 +21136,7 @@
       </c>
       <c r="G372" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H372" t="inlineStr">
@@ -21156,7 +21190,7 @@
       </c>
       <c r="G373" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H373" t="inlineStr">
@@ -21216,7 +21250,7 @@
       </c>
       <c r="G374" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H374" t="inlineStr">
@@ -21270,7 +21304,7 @@
       </c>
       <c r="G375" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H375" t="inlineStr">
@@ -21324,7 +21358,7 @@
       </c>
       <c r="G376" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>PRAMOD-JAIPUR</t>
         </is>
       </c>
       <c r="H376" t="inlineStr">
@@ -21378,7 +21412,7 @@
       </c>
       <c r="G377" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>PRAMOD-JAIPUR</t>
         </is>
       </c>
       <c r="H377" t="inlineStr">
@@ -21432,7 +21466,7 @@
       </c>
       <c r="G378" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H378" t="inlineStr">
@@ -21492,7 +21526,7 @@
       </c>
       <c r="G379" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H379" t="inlineStr">
@@ -21552,7 +21586,7 @@
       </c>
       <c r="G380" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H380" t="inlineStr">
@@ -21606,7 +21640,7 @@
       </c>
       <c r="G381" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H381" t="inlineStr">
@@ -21660,7 +21694,7 @@
       </c>
       <c r="G382" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H382" t="inlineStr">
@@ -21714,7 +21748,7 @@
       </c>
       <c r="G383" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H383" t="inlineStr">
@@ -21768,7 +21802,7 @@
       </c>
       <c r="G384" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H384" t="inlineStr">
@@ -21828,7 +21862,7 @@
       </c>
       <c r="G385" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>PRAMOD-JAIPUR</t>
         </is>
       </c>
       <c r="H385" t="inlineStr">
@@ -21882,7 +21916,7 @@
       </c>
       <c r="G386" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H386" t="inlineStr">
@@ -21936,7 +21970,7 @@
       </c>
       <c r="G387" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>PRAMOD-JAIPUR</t>
         </is>
       </c>
       <c r="H387" t="inlineStr">
@@ -21990,7 +22024,7 @@
       </c>
       <c r="G388" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H388" t="inlineStr">
@@ -22044,7 +22078,7 @@
       </c>
       <c r="G389" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>PRAMOD-JAIPUR</t>
         </is>
       </c>
       <c r="H389" t="inlineStr">
@@ -22098,7 +22132,7 @@
       </c>
       <c r="G390" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H390" t="inlineStr">
@@ -22115,7 +22149,7 @@
         <v>487881</v>
       </c>
       <c r="K390" t="n">
-        <v>3644</v>
+        <v>4567</v>
       </c>
       <c r="L390" t="inlineStr">
         <is>
@@ -22128,7 +22162,7 @@
         </is>
       </c>
       <c r="N390" t="n">
-        <v>291.52</v>
+        <v>365.36</v>
       </c>
     </row>
     <row r="391">
@@ -22158,7 +22192,7 @@
       </c>
       <c r="G391" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H391" t="inlineStr">
@@ -22212,7 +22246,7 @@
       </c>
       <c r="G392" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H392" t="inlineStr">
@@ -22266,7 +22300,7 @@
       </c>
       <c r="G393" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H393" t="inlineStr">
@@ -22320,7 +22354,7 @@
       </c>
       <c r="G394" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H394" t="inlineStr">
@@ -22374,7 +22408,7 @@
       </c>
       <c r="G395" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H395" t="inlineStr">
@@ -22428,7 +22462,7 @@
       </c>
       <c r="G396" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H396" t="inlineStr">

</xml_diff>

<commit_message>
Some Changes in Slice-CC-2
</commit_message>
<xml_diff>
--- a/media/SLICE/Billing/FEB 22/SLICE BILLING.xlsx
+++ b/media/SLICE/Billing/FEB 22/SLICE BILLING.xlsx
@@ -2784,7 +2784,7 @@
         <v>79941</v>
       </c>
       <c r="F43" t="n">
-        <v>79941</v>
+        <v>8961</v>
       </c>
       <c r="G43" t="inlineStr">
         <is>
@@ -2809,12 +2809,16 @@
       </c>
       <c r="L43" t="inlineStr">
         <is>
-          <t>PART PAID</t>
-        </is>
-      </c>
-      <c r="M43" t="inlineStr"/>
+          <t>NM</t>
+        </is>
+      </c>
+      <c r="M43" t="inlineStr">
+        <is>
+          <t>7%</t>
+        </is>
+      </c>
       <c r="N43" t="n">
-        <v>0</v>
+        <v>627.27</v>
       </c>
     </row>
     <row r="44">
@@ -5780,7 +5784,7 @@
         <v>56261</v>
       </c>
       <c r="F97" t="n">
-        <v>19743</v>
+        <v>11992</v>
       </c>
       <c r="G97" t="inlineStr">
         <is>
@@ -5805,12 +5809,16 @@
       </c>
       <c r="L97" t="inlineStr">
         <is>
-          <t>PART PAID</t>
-        </is>
-      </c>
-      <c r="M97" t="inlineStr"/>
+          <t>SB</t>
+        </is>
+      </c>
+      <c r="M97" t="inlineStr">
+        <is>
+          <t>8%</t>
+        </is>
+      </c>
       <c r="N97" t="n">
-        <v>0</v>
+        <v>959.36</v>
       </c>
     </row>
     <row r="98">
@@ -9689,12 +9697,16 @@
       </c>
       <c r="L167" t="inlineStr">
         <is>
-          <t>PART PAID</t>
-        </is>
-      </c>
-      <c r="M167" t="inlineStr"/>
+          <t>SB</t>
+        </is>
+      </c>
+      <c r="M167" t="inlineStr">
+        <is>
+          <t>7%</t>
+        </is>
+      </c>
       <c r="N167" t="n">
-        <v>0</v>
+        <v>933.3099999999999</v>
       </c>
     </row>
     <row r="168">

</xml_diff>